<commit_message>
add machine learn module.
</commit_message>
<xml_diff>
--- a/model/三焦点项目数据V1.0.xlsx
+++ b/model/三焦点项目数据V1.0.xlsx
@@ -5857,7 +5857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
       <selection activeCell="C104" sqref="C104"/>
@@ -11293,114 +11293,57 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="0" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="B103" s="0" t="inlineStr">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
         <is>
           <t>男</t>
         </is>
       </c>
-      <c r="C103" s="0" t="inlineStr">
+      <c r="C103" t="inlineStr">
         <is>
           <t>博士</t>
         </is>
       </c>
-      <c r="D103" s="0" t="inlineStr">
-        <is>
-          <t>高</t>
-        </is>
-      </c>
-      <c r="E103" s="0" t="inlineStr">
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>高</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
         <is>
           <t>无</t>
         </is>
       </c>
-      <c r="F103" s="0" t="inlineStr">
+      <c r="F103" t="inlineStr">
         <is>
           <t>一甲</t>
         </is>
       </c>
-      <c r="G103" s="0" t="inlineStr">
-        <is>
-          <t>有</t>
-        </is>
-      </c>
-      <c r="H103" s="0" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="I103" s="0" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="J103" s="0" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="K103" s="0" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>男</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>高中</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>高</t>
-        </is>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>无</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>一甲</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>无</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>是</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>有</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>是</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
         <is>
           <t>是</t>
         </is>

</xml_diff>